<commit_message>
Addeding new charts and scripts
</commit_message>
<xml_diff>
--- a/twitter_data/MediaAnalysisCharts.xlsx
+++ b/twitter_data/MediaAnalysisCharts.xlsx
@@ -56,13 +56,7 @@
     <t xml:space="preserve"> 42/136</t>
   </si>
   <si>
-    <t>Popular</t>
-  </si>
-  <si>
     <t>Percentage of Medias ___________________________________________</t>
-  </si>
-  <si>
-    <t>Unpopular</t>
   </si>
   <si>
     <t>All</t>
@@ -99,6 +93,12 @@
   </si>
   <si>
     <t>Number of Tweets with Media (Photo or Video)</t>
+  </si>
+  <si>
+    <t>Baseline ( &lt; 5 RT )</t>
+  </si>
+  <si>
+    <t>Popular ( &gt;= 5 RT )</t>
   </si>
 </sst>
 </file>
@@ -409,33 +409,6 @@
                   <a:p>
                     <a:r>
                       <a:rPr lang="en-US"/>
-                      <a:t>15.27%</a:t>
-                    </a:r>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="3"/>
-              <c:layout/>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:r>
-                      <a:rPr lang="en-US"/>
                       <a:t>17.12%</a:t>
                     </a:r>
                   </a:p>
@@ -511,19 +484,16 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$H$7:$K$7</c:f>
+              <c:f>Sheet1!$H$7:$J$7</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>Popular</c:v>
+                  <c:v>Popular ( &gt;= 5 RT )</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Unpopular</c:v>
+                  <c:v>Baseline ( &lt; 5 RT )</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Zero</c:v>
-                </c:pt>
-                <c:pt idx="3">
                   <c:v>All</c:v>
                 </c:pt>
               </c:strCache>
@@ -531,10 +501,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$8:$K$8</c:f>
+              <c:f>Sheet1!$H$8:$J$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>42.0</c:v>
                 </c:pt>
@@ -542,9 +512,6 @@
                   <c:v>1473.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1165.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
                   <c:v>1515.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -669,33 +636,6 @@
                   <a:p>
                     <a:r>
                       <a:rPr lang="en-US"/>
-                      <a:t>84.73%</a:t>
-                    </a:r>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="3"/>
-              <c:layout/>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:r>
-                      <a:rPr lang="en-US"/>
                       <a:t>82.88%</a:t>
                     </a:r>
                   </a:p>
@@ -771,19 +711,16 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$H$7:$K$7</c:f>
+              <c:f>Sheet1!$H$7:$J$7</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>Popular</c:v>
+                  <c:v>Popular ( &gt;= 5 RT )</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Unpopular</c:v>
+                  <c:v>Baseline ( &lt; 5 RT )</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Zero</c:v>
-                </c:pt>
-                <c:pt idx="3">
                   <c:v>All</c:v>
                 </c:pt>
               </c:strCache>
@@ -791,10 +728,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$9:$K$9</c:f>
+              <c:f>Sheet1!$H$9:$J$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>73.0</c:v>
                 </c:pt>
@@ -802,9 +739,6 @@
                   <c:v>7262.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6465.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
                   <c:v>7335.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -821,11 +755,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="100"/>
-        <c:axId val="-2094162336"/>
-        <c:axId val="-2115083232"/>
+        <c:axId val="-2082829216"/>
+        <c:axId val="-2082828368"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2094162336"/>
+        <c:axId val="-2082829216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -868,7 +802,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2115083232"/>
+        <c:crossAx val="-2082828368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -876,7 +810,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2115083232"/>
+        <c:axId val="-2082828368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -913,7 +847,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2094162336"/>
+        <c:crossAx val="-2082829216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1086,7 +1020,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$K$7</c:f>
+              <c:f>Sheet1!$J$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1222,7 +1156,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$K$8:$K$9</c:f>
+              <c:f>Sheet1!$J$8:$J$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -2868,8 +2802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D8" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2880,7 +2814,7 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
@@ -2897,7 +2831,7 @@
       </c>
       <c r="D3" s="1"/>
       <c r="M3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
@@ -2919,7 +2853,7 @@
         <v>1</v>
       </c>
       <c r="O5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
@@ -2945,16 +2879,16 @@
         <v>0.13410839999999999</v>
       </c>
       <c r="H7" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="I7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J7" t="s">
+        <v>11</v>
+      </c>
+      <c r="L7" t="s">
         <v>12</v>
-      </c>
-      <c r="J7" t="s">
-        <v>14</v>
-      </c>
-      <c r="K7" t="s">
-        <v>13</v>
       </c>
       <c r="M7" t="s">
         <v>4</v>
@@ -2962,10 +2896,10 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H8">
         <v>42</v>
@@ -2974,16 +2908,16 @@
         <v>1473</v>
       </c>
       <c r="J8">
+        <v>1515</v>
+      </c>
+      <c r="L8">
         <v>1165</v>
-      </c>
-      <c r="K8">
-        <v>1515</v>
       </c>
       <c r="M8" t="s">
         <v>1</v>
       </c>
       <c r="O8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
@@ -2991,11 +2925,11 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D9" s="1"/>
       <c r="G9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H9">
         <v>73</v>
@@ -3004,10 +2938,10 @@
         <v>7262</v>
       </c>
       <c r="J9">
+        <v>7335</v>
+      </c>
+      <c r="L9">
         <v>6465</v>
-      </c>
-      <c r="K9">
-        <v>7335</v>
       </c>
       <c r="M9" t="s">
         <v>3</v>
@@ -3024,7 +2958,7 @@
         <v>0.14763960000000001</v>
       </c>
       <c r="G10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H10">
         <v>115</v>
@@ -3033,13 +2967,13 @@
         <v>8735</v>
       </c>
       <c r="J10">
+        <v>8850</v>
+      </c>
+      <c r="L10">
         <v>7630</v>
       </c>
-      <c r="K10">
-        <v>8850</v>
-      </c>
       <c r="M10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
@@ -3047,7 +2981,7 @@
         <v>6</v>
       </c>
       <c r="G11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H11" s="1">
         <v>0.36521740000000003</v>
@@ -3056,16 +2990,16 @@
         <v>0.1686319</v>
       </c>
       <c r="J11" s="1">
+        <v>0.17118639999999999</v>
+      </c>
+      <c r="L11" s="1">
         <v>0.15268680000000001</v>
-      </c>
-      <c r="K11" s="1">
-        <v>0.17118639999999999</v>
       </c>
       <c r="M11" t="s">
         <v>1</v>
       </c>
       <c r="O11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
@@ -3121,7 +3055,7 @@
         <v>1</v>
       </c>
       <c r="O17" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="13:16" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
cleaned up a bit and added the Media Analysis Graphs
</commit_message>
<xml_diff>
--- a/twitter_data/MediaAnalysisCharts.xlsx
+++ b/twitter_data/MediaAnalysisCharts.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="28720" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="35320" windowHeight="19740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -343,7 +343,7 @@
                       <a:rPr lang="en-US" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0">
                         <a:effectLst/>
                       </a:rPr>
-                      <a:t>36.52%</a:t>
+                      <a:t>16.86%</a:t>
                     </a:r>
                     <a:r>
                       <a:rPr lang="en-US" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
@@ -377,7 +377,7 @@
                       <a:rPr lang="en-US" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0">
                         <a:effectLst/>
                       </a:rPr>
-                      <a:t>16.86%</a:t>
+                      <a:t>36.52%</a:t>
                     </a:r>
                     <a:r>
                       <a:rPr lang="en-US" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
@@ -488,10 +488,10 @@
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>Popular ( &gt;= 5 RT )</c:v>
+                  <c:v>Baseline ( &lt; 5 RT )</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Baseline ( &lt; 5 RT )</c:v>
+                  <c:v>Popular ( &gt;= 5 RT )</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>All</c:v>
@@ -506,10 +506,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>42.0</c:v>
+                  <c:v>1473.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1473.0</c:v>
+                  <c:v>42.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1515.0</c:v>
@@ -582,7 +582,7 @@
                   <a:p>
                     <a:r>
                       <a:rPr lang="en-US"/>
-                      <a:t>63.48%</a:t>
+                      <a:t>83.14%</a:t>
                     </a:r>
                   </a:p>
                 </c:rich>
@@ -609,7 +609,7 @@
                   <a:p>
                     <a:r>
                       <a:rPr lang="en-US"/>
-                      <a:t>83.14%</a:t>
+                      <a:t>63.48%</a:t>
                     </a:r>
                   </a:p>
                 </c:rich>
@@ -715,10 +715,10 @@
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>Popular ( &gt;= 5 RT )</c:v>
+                  <c:v>Baseline ( &lt; 5 RT )</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Baseline ( &lt; 5 RT )</c:v>
+                  <c:v>Popular ( &gt;= 5 RT )</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>All</c:v>
@@ -733,10 +733,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>73.0</c:v>
+                  <c:v>7262.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7262.0</c:v>
+                  <c:v>73.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>7335.0</c:v>
@@ -755,11 +755,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="100"/>
-        <c:axId val="-2121581888"/>
-        <c:axId val="-2121578960"/>
+        <c:axId val="-2056430800"/>
+        <c:axId val="-2056427872"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2121581888"/>
+        <c:axId val="-2056430800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -802,7 +802,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2121578960"/>
+        <c:crossAx val="-2056427872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -810,7 +810,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2121578960"/>
+        <c:axId val="-2056427872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -847,7 +847,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2121581888"/>
+        <c:crossAx val="-2056430800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1366,7 +1366,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.0455028726338259"/>
+          <c:y val="0.127280701754386"/>
+          <c:w val="0.927611391742574"/>
+          <c:h val="0.706081410876272"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="percentStacked"/>
@@ -1430,23 +1440,67 @@
               <c:layout/>
               <c:tx>
                 <c:rich>
-                  <a:bodyPr/>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                    <a:spAutoFit/>
+                  </a:bodyPr>
                   <a:lstStyle/>
                   <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="75000"/>
+                            <a:lumOff val="25000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
                     <a:r>
-                      <a:rPr lang="en-US" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                      <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="0">
                         <a:effectLst/>
                       </a:rPr>
-                      <a:t>36.52%</a:t>
+                      <a:t>16.86%</a:t>
                     </a:r>
                     <a:r>
-                      <a:rPr lang="en-US" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
+                      <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
                       <a:t> </a:t>
                     </a:r>
-                    <a:endParaRPr lang="en-US" b="1"/>
+                    <a:endParaRPr lang="en-US" sz="1600" b="1"/>
                   </a:p>
                 </c:rich>
               </c:tx>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="75000"/>
+                          <a:lumOff val="25000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
@@ -1464,23 +1518,67 @@
               <c:layout/>
               <c:tx>
                 <c:rich>
-                  <a:bodyPr/>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                    <a:spAutoFit/>
+                  </a:bodyPr>
                   <a:lstStyle/>
                   <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="75000"/>
+                            <a:lumOff val="25000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
                     <a:r>
-                      <a:rPr lang="en-US" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                      <a:rPr lang="en-US" sz="1800" b="1" i="0" u="none" strike="noStrike" baseline="0">
                         <a:effectLst/>
                       </a:rPr>
-                      <a:t>16.86%</a:t>
+                      <a:t>36.52%</a:t>
                     </a:r>
                     <a:r>
-                      <a:rPr lang="en-US" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
+                      <a:rPr lang="en-US" sz="1800" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
                       <a:t> </a:t>
                     </a:r>
-                    <a:endParaRPr lang="en-US" b="1"/>
+                    <a:endParaRPr lang="en-US" sz="1800" b="1"/>
                   </a:p>
                 </c:rich>
               </c:tx>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="75000"/>
+                          <a:lumOff val="25000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
@@ -1507,7 +1605,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="7700" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -1555,10 +1653,10 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>Popular ( &gt;= 5 RT )</c:v>
+                  <c:v>Baseline ( &lt; 5 RT )</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Baseline ( &lt; 5 RT )</c:v>
+                  <c:v>Popular ( &gt;= 5 RT )</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1570,10 +1668,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>42.0</c:v>
+                  <c:v>1473.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1473.0</c:v>
+                  <c:v>42.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1643,7 +1741,7 @@
                   <a:p>
                     <a:r>
                       <a:rPr lang="en-US"/>
-                      <a:t>63.48%</a:t>
+                      <a:t>83.14%</a:t>
                     </a:r>
                   </a:p>
                 </c:rich>
@@ -1670,7 +1768,7 @@
                   <a:p>
                     <a:r>
                       <a:rPr lang="en-US"/>
-                      <a:t>83.14%</a:t>
+                      <a:t>63.48%</a:t>
                     </a:r>
                   </a:p>
                 </c:rich>
@@ -1701,7 +1799,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -1749,10 +1847,10 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>Popular ( &gt;= 5 RT )</c:v>
+                  <c:v>Baseline ( &lt; 5 RT )</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Baseline ( &lt; 5 RT )</c:v>
+                  <c:v>Popular ( &gt;= 5 RT )</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1764,10 +1862,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>73.0</c:v>
+                  <c:v>7262.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7262.0</c:v>
+                  <c:v>73.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1783,11 +1881,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="100"/>
-        <c:axId val="-2043402752"/>
-        <c:axId val="-2043124064"/>
+        <c:axId val="-2037035024"/>
+        <c:axId val="-2037032096"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2043402752"/>
+        <c:axId val="-2037035024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1815,7 +1913,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1830,7 +1928,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2043124064"/>
+        <c:crossAx val="-2037032096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1838,7 +1936,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2043124064"/>
+        <c:axId val="-2037032096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1875,7 +1973,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2043402752"/>
+        <c:crossAx val="-2037035024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1889,7 +1987,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.120958642305634"/>
+          <c:y val="0.906669659713589"/>
+          <c:w val="0.767044509652873"/>
+          <c:h val="0.0728625040291016"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1903,7 +2010,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -4043,13 +4150,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C5" workbookViewId="0">
-      <selection activeCell="O42" sqref="O42"/>
+    <sheetView tabSelected="1" topLeftCell="H3" workbookViewId="0">
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="7" max="7" width="37.6640625" customWidth="1"/>
+    <col min="13" max="13" width="10.83203125" customWidth="1"/>
     <col min="16" max="16" width="15" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4120,10 +4228,10 @@
         <v>0.13410839999999999</v>
       </c>
       <c r="H7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" t="s">
         <v>24</v>
-      </c>
-      <c r="I7" t="s">
-        <v>23</v>
       </c>
       <c r="J7" t="s">
         <v>11</v>
@@ -4143,10 +4251,10 @@
         <v>22</v>
       </c>
       <c r="H8">
+        <v>1473</v>
+      </c>
+      <c r="I8">
         <v>42</v>
-      </c>
-      <c r="I8">
-        <v>1473</v>
       </c>
       <c r="J8">
         <v>1515</v>
@@ -4173,10 +4281,10 @@
         <v>17</v>
       </c>
       <c r="H9">
+        <v>7262</v>
+      </c>
+      <c r="I9">
         <v>73</v>
-      </c>
-      <c r="I9">
-        <v>7262</v>
       </c>
       <c r="J9">
         <v>7335</v>
@@ -4202,10 +4310,10 @@
         <v>16</v>
       </c>
       <c r="H10">
+        <v>8735</v>
+      </c>
+      <c r="I10">
         <v>115</v>
-      </c>
-      <c r="I10">
-        <v>8735</v>
       </c>
       <c r="J10">
         <v>8850</v>
@@ -4225,10 +4333,10 @@
         <v>15</v>
       </c>
       <c r="H11" s="1">
+        <v>0.1686319</v>
+      </c>
+      <c r="I11" s="1">
         <v>0.36521740000000003</v>
-      </c>
-      <c r="I11" s="1">
-        <v>0.1686319</v>
       </c>
       <c r="J11" s="1">
         <v>0.17118639999999999</v>

</xml_diff>